<commit_message>
fixing some issues and uploading new files
</commit_message>
<xml_diff>
--- a/Documents/Model/Acceptance tests.xlsx
+++ b/Documents/Model/Acceptance tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\School\SADNA\Workshop-On-Software-Engineering-Project-2019\Documents\Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF3B3B9-A412-4084-BED4-06C75CD38D82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C0685A-53D3-4C9A-891D-32C9A9B042A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" xr2:uid="{1CA65076-1370-4905-AE0F-4695E8F49515}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CA65076-1370-4905-AE0F-4695E8F49515}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="114">
   <si>
     <t>data</t>
   </si>
@@ -53,9 +53,6 @@
     <t>המערכת תבקש מהמשתמש להכניס ערך לא שלילי כפרמטר סינון</t>
   </si>
   <si>
-    <t>סינון מוצרים לפי סינון מוצרים לפי טווח מחירים לא ולידי - 500$-</t>
-  </si>
-  <si>
     <t>סינון מוצרים לפי דירוג מוצר ולידי - 3</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>המשתמש בוחר להוסיף לעגלה שלו מוצר עם מזהה id_1, כאשר id_1 הוא מזהה של מוצר שלא קיים במערכת. עגלת הקניות של המשתמש ריקה</t>
   </si>
   <si>
-    <t>עגלת המשתמש מכילה את המוצרים id_1, id_3, id_3 בלבד. המשתמש בוחר לערוך את העגלה ומסיר ממנה את המוצ Id_2</t>
-  </si>
-  <si>
     <t>עגלת המשתמש מכילה את המוצרים id_1, id_3 בלבד</t>
   </si>
   <si>
@@ -146,15 +140,9 @@
     <t>המשתמש לא מחובר למערכת</t>
   </si>
   <si>
-    <t>המשתמש מזוהה כמנוי של המערכת ואינו בעל חנות. הוא מבקש לפתוח את החנות id_1</t>
-  </si>
-  <si>
     <t>המשתמש לא מזוהה כמנוי של המערכת. הוא מבקש לפתוח את החנות id_1</t>
   </si>
   <si>
-    <t>המערכת מחזירה הודעה על כך הכדיי לפתוח חנות המשתמש חייב להיות מנוי של המערכת. לא נפתחת חנות id_1</t>
-  </si>
-  <si>
     <t>המשתמש מזוהה כבעל החנות. הוא מסיר את המוצר id_1 אשר קיים בחנות</t>
   </si>
   <si>
@@ -185,9 +173,6 @@
     <t>המערכת מחזירה הודעה על זה שרק בעל החנות אשר מינה את id_1 יכול להסיר אותו. Id_1 נותר בעל החנות</t>
   </si>
   <si>
-    <t>מנוי id_1 נהפך למנהל חנות נוסף שיש לו זכויות לניהול החנות</t>
-  </si>
-  <si>
     <t>המערכת מחזירה הודעה על זה שרק בעל החנות יכול למנות מנהל חנות נוסף. Id_2 נותר בעל החנות היחידי</t>
   </si>
   <si>
@@ -227,9 +212,6 @@
     <t>המערכת מציגה למשתמש הודעה על כך שעל מנת להסיר מוצר הוא צריך הרשאות להסרת מוצר. המוצר נותר במלאי</t>
   </si>
   <si>
-    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר קיים במערכת id_1</t>
-  </si>
-  <si>
     <t>המשתמש id_1 מוסר מהמערכת</t>
   </si>
   <si>
@@ -242,21 +224,12 @@
     <t>נפתחה החנות id_1. המשתמש מוגדר כבעל חנות</t>
   </si>
   <si>
-    <t>גביית כספים</t>
-  </si>
-  <si>
     <t>המערכת מחזירה אישור כי העסקה בוצעה בהצלחה</t>
   </si>
   <si>
     <t>המערכת מחזירה הודעת שגיאה על כך שיש סתירה בעסקה למדיניות החנות, ומודיעה שהעסקה לא התבצעה</t>
   </si>
   <si>
-    <t>אספקת מוצרים</t>
-  </si>
-  <si>
-    <t>המשתמש מבקש לבצע לרכוש מוצרים והעסקה עומדת בחוקי המדיניות שהגדיר בעל החנות</t>
-  </si>
-  <si>
     <t>המשתמש מבקש לבצע לרכוש מוצרים וקיימת סתירה למדיניות אותה הגדיר בעל החנות</t>
   </si>
   <si>
@@ -272,30 +245,18 @@
     <t>המשתמש מבקש להזמין אספקה עבור סל הקניות שלו על עסקה שלא אושר עליה תשלום ממערכת הגבייה</t>
   </si>
   <si>
-    <t>המשתמש הוא אורח, הוא מנסה להיכנס עם פרטי משתמש אשר לא קיים במערכת</t>
-  </si>
-  <si>
-    <t>המערכת מציגה למשתמש הודעה על כך הצליח להתחבר בהצלחה והמשתמש מוגדר כמנוי במערכת</t>
-  </si>
-  <si>
     <t>המשתמש הוא אורח, הוא מנסה להיכנס עם פרטי משתמש אשר כן קיים במערכת</t>
   </si>
   <si>
     <t>המערכת מציגה למשתמש הודעה על כך ששם המשתמש איתו מבקש להתחבר כבר קיים</t>
   </si>
   <si>
-    <t>המשתמש אורח, הוא מנסה להשתמש עם שם משתמש וססמא נכונה</t>
-  </si>
-  <si>
     <t>המתשמש מזוהה כמנוי שמתאים לשם המשתמש שהזין</t>
   </si>
   <si>
     <t>המשתמש אורח, הוא מנסה להשתמש עם שם משתמש שלא קיים</t>
   </si>
   <si>
-    <t>המשתמש אורח, הוא מנסה להשתמש עם שם משתמש שקיים במערכת עם ססמא שגויה</t>
-  </si>
-  <si>
     <t>המערכת מחזירה הודעת שגיאה על כך אחד פרטי המשתמש שגויים</t>
   </si>
   <si>
@@ -323,9 +284,6 @@
     <t>המערכת מחזירה הודעה על זה שרק בעל החנות עם הרשאות להוסיף ולהסיר עובדים רשאי להסיר עובדים</t>
   </si>
   <si>
-    <t>משתמש מזוהה כבעל חנות ויש לו הרשאות להוסיף ולהסיר עובדים. והמשתמש id_1 שאותו רוצים למנות מזוהה כמנוי. יש ממנה יחיד לחנות</t>
-  </si>
-  <si>
     <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר קיים במערכת id_1 ומוגדר כבעל החנות עם חנויות id_2 ו id_3</t>
   </si>
   <si>
@@ -335,7 +293,85 @@
     <t>משתמש id_1 מזוהה כבעל חנות אשר מונה על ידי משתמש id_2. המשתמש id_2 מנסה למנות לבעל החנות את Id_1</t>
   </si>
   <si>
-    <t>המערכת מחזירה הודעה על כך שבעל חנות לא יכול להוסיף את מי שהוסיף אותו</t>
+    <t>המשתמש הוא אורח, הוא מנסה להירשם עם פרטי משתמש אשר לא קיים במערכת וסיסמה חוקית</t>
+  </si>
+  <si>
+    <t>המשתמש הוא אורח, הוא מנסה להיכנס עם פרטי משתמש אשר לא קיים במערכת אך עם סיסמה שאינה חוקית</t>
+  </si>
+  <si>
+    <t>המערכת מציגה למשתמש הודעה על כך שהסיסמה אינה חוקית והרישום נכשל</t>
+  </si>
+  <si>
+    <t>המשתמש אורח, הוא מנסה להשתמש עם שם משתמש וסיסמא נכונים</t>
+  </si>
+  <si>
+    <t>המשתמש אורח, הוא מנסה להשתמש עם שם משתמש שקיים במערכת אך עם ססמא שגויה</t>
+  </si>
+  <si>
+    <t>חיפוש מוצר לפי מילות מפתח - 'candle'</t>
+  </si>
+  <si>
+    <t>המערכת תציג למשתמש את כל המוצרים שהמילה candle מקושרת אליהם</t>
+  </si>
+  <si>
+    <t>סינון מוצרים לפי טווח מחירים לא ולידי - 500$-</t>
+  </si>
+  <si>
+    <t>עגלת המשתמש מכילה את המוצרים id_1, id_2, id_3 בלבד. המשתמש בוחר לערוך את העגלה ומסיר ממנה את המוצר Id_2</t>
+  </si>
+  <si>
+    <t>עגלת המשתמש מכילה את המוצרים id_1, id_2 בלבד. המשתמש בוחר לערוך את העגלה ולהוסיף עוד 2 פריטים מהמוצר id_1</t>
+  </si>
+  <si>
+    <t>עגלת המשתמש מכילה 3 פריטים של המוצר Id_1 ופריט אחד מהמוצר Id_2</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אשר לא קיימת במערכת</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שכדי לפתוח חנות המשתמש חייב להיות מנוי של המערכת. לא נפתחת חנות id_1</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שכבר קיימת חנות עם שם זה במערכת. לא נפתחת חנות id_1</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אשר קיימת כבר במערכת</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שבעל חנות לא יכול להוסיף את מי שהוסיף אותו (אין מעגליות)</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות והמשתמש id_1 שאותו רוצים למנות מזוהה כמנוי, מבקשים הרשאה לערוך מוצרים. יש ממנה יחיד לחנות</t>
+  </si>
+  <si>
+    <t>מנוי id_1 נהפך למנהל חנות נוסף שיש לו זכויות לערוך מוצרי החנות</t>
+  </si>
+  <si>
+    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר קיים במערכת id_1 (ולו אין קניות או מכירות בתהליך)</t>
+  </si>
+  <si>
+    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר קיים במערכת id_1 שהינו בעל חנות יחיד</t>
+  </si>
+  <si>
+    <t>המשתמש id_1 מוסר מהמערכת וכן חנותו והמוצרים אותם הוא מוכר נמחקים מהמערכת</t>
+  </si>
+  <si>
+    <t>המשתמש מבקש לבצע לרכוש מוצרים והעסקה עומדת בחוקי המדיניות שהגדיר בעל החנות אך המשתמש הזין פרטי תשלום שאינם ולידיים</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי התשלום נכשל ומציעה למשתמש להזין פרטי התשלום בשנית</t>
+  </si>
+  <si>
+    <t>המשתמש מבקש לבצע לרכוש מוצרים והעסקה עומדת בחוקי המדיניות שהגדיר בעל החנות. כן, המשתמש הזין פרטי תשלום ולידיים.</t>
+  </si>
+  <si>
+    <t>המשתמש מבקש להזמין אספקה עבור סל הקניות שלו על עסקה שקיים לה אישור תשלום ממערכת הגבייה אך מזין כתובת שחברת האספקה לא מספקת אליה</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעת שגיאה על כך שלא ניתן להזמין אספקה עבור כתובת זו ומציעה למשתמש להזין כתובת אחרת</t>
+  </si>
+  <si>
+    <t>המערכת מציגה למשתמש הודעה על כך שהצליח להירשם בהצלחה והמשתמש מוגדר כמנוי במערכת, אך אינו מחובר</t>
   </si>
 </sst>
 </file>
@@ -429,8 +465,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6CFC1F84-449F-47ED-BBEA-4EF5BEC0A93A}" name="Table1" displayName="Table1" ref="B1:E50" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="B1:E50" xr:uid="{AD44D35B-AAB7-4FAB-8348-524CACD0E48F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6CFC1F84-449F-47ED-BBEA-4EF5BEC0A93A}" name="Table1" displayName="Table1" ref="B1:E57" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B1:E57" xr:uid="{AD44D35B-AAB7-4FAB-8348-524CACD0E48F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A7C70BDA-E6BF-4FDC-92ED-77951EB0BE2A}" name="expected result" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0AF91C84-E078-467D-8BAA-5AAC4C6F1F02}" name="data" dataDxfId="2"/>
@@ -738,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB44C02-4CA2-465F-A9FE-5F1D45ACF731}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -778,10 +814,10 @@
     </row>
     <row r="3" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -792,10 +828,10 @@
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D4" s="3">
         <v>2</v>
@@ -806,27 +842,27 @@
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D5" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="3">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D6" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="3">
         <v>2.2999999999999998</v>
@@ -834,626 +870,724 @@
     </row>
     <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D7" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" s="3">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="D8" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" s="3">
-        <v>2.5</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="D9" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3">
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D10" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="3">
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="D11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" s="3">
         <v>2.5</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D12" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="3">
         <v>2.5</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B13" s="3" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="D13" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" s="3">
         <v>2.5</v>
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="D14" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E14" s="3">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>2.5</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="D15" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E15" s="3">
-        <v>2.6</v>
-      </c>
+        <v>2.5</v>
+      </c>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D16" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3">
         <v>2.6</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" ht="58" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
         <v>2.7</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="3">
-        <v>2</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="D20" s="3">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2.7</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D21" s="3">
-        <v>2</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="3">
-        <v>2</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="3">
-        <v>1</v>
-      </c>
-      <c r="E24" s="3">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="3">
-        <v>2</v>
-      </c>
-      <c r="E25" s="3">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="3">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3">
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" s="3">
         <v>3.2</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="3">
-        <v>2</v>
-      </c>
-      <c r="E27" s="3">
+    <row r="31" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
         <v>3.2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="3">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B29" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="3">
-        <v>2</v>
-      </c>
-      <c r="E29" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="3">
-        <v>1</v>
-      </c>
-      <c r="E30" s="3">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="3">
-        <v>2</v>
-      </c>
-      <c r="E31" s="3">
-        <v>4.3</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="D32" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E32" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="3">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3">
         <v>4.3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B33" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="3">
-        <v>4</v>
-      </c>
-      <c r="E33" s="3">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="3">
-        <v>1</v>
-      </c>
-      <c r="E34" s="3">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B35" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D35" s="3">
         <v>2</v>
       </c>
       <c r="E35" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="D36" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E36" s="3">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="D37" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E37" s="3">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="D38" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E38" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D39" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B40" s="1" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D40" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D41" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B42" s="3" t="s">
-        <v>64</v>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B42" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="D42" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E42" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B43" s="3" t="s">
-        <v>63</v>
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B43" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D43" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E43" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D44" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="3">
-        <v>6.2</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D45" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B46" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="3">
+        <v>2</v>
+      </c>
+      <c r="E46" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B47" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" s="3">
+        <v>3</v>
+      </c>
+      <c r="E47" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
         <v>6.2</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B46" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="3">
-        <v>3</v>
-      </c>
-      <c r="E46" s="3">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D47" s="3">
-        <v>1</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B48" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" s="3">
-        <v>2</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B49" s="1" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="D49" s="3">
-        <v>1</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="E49" s="3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B50" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D50" s="3">
-        <v>2</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>73</v>
+        <v>3</v>
+      </c>
+      <c r="E50" s="3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" s="3">
+        <v>3</v>
+      </c>
+      <c r="E51" s="3">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" s="3">
+        <v>2</v>
+      </c>
+      <c r="E53" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B54" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54" s="3">
+        <v>3</v>
+      </c>
+      <c r="E54" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B55" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" s="3">
+        <v>1</v>
+      </c>
+      <c r="E55" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B56" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" s="3">
+        <v>2</v>
+      </c>
+      <c r="E56" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="3">
+        <v>3</v>
+      </c>
+      <c r="E57" s="3">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>